<commit_message>
Latest version attempting to run conda
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -22,25 +22,25 @@
     <t>Opt Portfolio with View</t>
   </si>
   <si>
-    <t>European Banks</t>
-  </si>
-  <si>
-    <t>EU High Yield Bonds</t>
-  </si>
-  <si>
-    <t>Emerging Asia Equity</t>
-  </si>
-  <si>
-    <t>Chinese Equity</t>
-  </si>
-  <si>
-    <t>Chinese Bonds</t>
-  </si>
-  <si>
     <t>Cash</t>
   </si>
   <si>
-    <t>1-5 years GILTS</t>
+    <t>US Equities</t>
+  </si>
+  <si>
+    <t>European Equities</t>
+  </si>
+  <si>
+    <t>EU High Yield</t>
+  </si>
+  <si>
+    <t>EU Corporate</t>
+  </si>
+  <si>
+    <t>Greek Gov</t>
+  </si>
+  <si>
+    <t>Euro Gov</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Renaming files to more easily understandable names
I renamed two files to make clearer what Input the received. One received our Excel file from Bberg-excel the other pulled data straight from Bberg's-database and was hence named the Official code.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user2\Documents\Python_files\Black_Litterman\Iolcus-Investments\Main\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADA285D-83BC-4D9C-8FCB-F8EBED72AAD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -67,11 +61,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,13 +72,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -127,31 +111,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -198,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,27 +203,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,24 +237,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -475,21 +412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,140 +427,139 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.8813380504120236E-19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.881338050412024e-19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.36779723959161792</v>
+      <c r="B3">
+        <v>0.3677972395916179</v>
       </c>
       <c r="C3">
-        <v>0.45526040389682071</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4552604038968207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>2.992458714920683E-2</v>
+      <c r="B4">
+        <v>0.02992458714920683</v>
       </c>
       <c r="C4">
-        <v>6.8091718501921236E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.06809171850192124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.12347964605337609</v>
+      <c r="B5">
+        <v>0.1234796460533761</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.29782338828919219</v>
+      <c r="B6">
+        <v>0.2978233882891922</v>
       </c>
       <c r="C6">
-        <v>0.36607090932068009</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3660709093206801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
-        <v>1.0904137530296589E-2</v>
+      <c r="B7">
+        <v>0.01090413753029659</v>
       </c>
       <c r="C7">
-        <v>9.0562902031226054E-19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9.056290203122605e-19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>2.6249614029891109E-17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.624961402989111e-17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
-        <v>4.5143928922989081E-2</v>
+      <c r="B9">
+        <v>0.04514392892298908</v>
       </c>
       <c r="C9">
-        <v>5.1178474679940397E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.0511784746799404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
-        <v>4.8843318133160438E-2</v>
+      <c r="B10">
+        <v>0.04884331813316044</v>
       </c>
       <c r="C10">
-        <v>2.3834511636659669E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.02383451163665967</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
-        <v>4.5091210520712383E-2</v>
+      <c r="B11">
+        <v>0.04509121052071238</v>
       </c>
       <c r="C11">
-        <v>3.556398196397785E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.03556398196397785</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>4.5622682215306743E-19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.562268221530674e-19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2">
-        <v>3.0992543809448578E-2</v>
+      <c r="B13">
+        <v>0.03099254380944858</v>
       </c>
       <c r="C13">
-        <v>2.2807684260096598E-19</v>
+        <v>2.28076842600966e-19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Doing a slight reoderning of files for declutering purposes
Relocated all non-main_code files into an archive folder to decluter workspace
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user2\Documents\Python_files\Black_Litterman\Iolcus-Investments\Main\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E3C0DB-B9D1-4AF3-BA12-04E52B54D076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Opt Portfolio</t>
   </si>
@@ -56,13 +62,16 @@
   </si>
   <si>
     <t>S&amp;P 500</t>
+  </si>
+  <si>
+    <t>Implied weights are same with Black Litterman weights since no view has been supplied yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +134,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -171,7 +188,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,9 +220,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,6 +272,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -412,14 +465,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -438,62 +493,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.3677972395916179</v>
+        <v>0.36779723959161792</v>
       </c>
       <c r="C3">
         <v>0.3677972307464058</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.02992458714920683</v>
+        <v>2.992458714920683E-2</v>
       </c>
       <c r="C4">
-        <v>0.02992461252661037</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>2.992461252661037E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.1234796460533761</v>
+        <v>0.12347964605337609</v>
       </c>
       <c r="C5">
         <v>0.1234796466906095</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.2978233882891922</v>
+        <v>0.29782338828919219</v>
       </c>
       <c r="C6">
-        <v>0.2978233793571007</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>0.29782337935710068</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.01090413753029659</v>
+        <v>1.0904137530296589E-2</v>
       </c>
       <c r="C7">
-        <v>0.01090413015614074</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>1.0904130156140741E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -504,40 +559,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.04514392892298908</v>
+        <v>4.5143928922989081E-2</v>
       </c>
       <c r="C9">
-        <v>0.04514393665358528</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>4.5143936653585279E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.04884331813316044</v>
+        <v>4.8843318133160438E-2</v>
       </c>
       <c r="C10">
-        <v>0.04884331010259938</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>4.8843310102599381E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.04509121052071238</v>
+        <v>4.5091210520712383E-2</v>
       </c>
       <c r="C11">
-        <v>0.04509121361603211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>4.5091213616032112E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -548,15 +603,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.03099254380944858</v>
+        <v>3.0992543809448578E-2</v>
       </c>
       <c r="C13">
-        <v>0.03099254015091614</v>
+        <v>3.099254015091614E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Something interactive is printed
First steps of untangling the printing of interactive elements
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user2\Documents\Python_files\Black_Litterman\Iolcus-Investments\Main\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E3C0DB-B9D1-4AF3-BA12-04E52B54D076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Opt Portfolio</t>
   </si>
@@ -62,16 +56,13 @@
   </si>
   <si>
     <t>S&amp;P 500</t>
-  </si>
-  <si>
-    <t>Implied weights are same with Black Litterman weights since no view has been supplied yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,14 +125,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -188,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -220,27 +203,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,24 +237,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -465,16 +412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -493,62 +438,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.36779723959161792</v>
+        <v>0.3677972395916179</v>
       </c>
       <c r="C3">
         <v>0.3677972307464058</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2.992458714920683E-2</v>
+        <v>0.02992458714920683</v>
       </c>
       <c r="C4">
-        <v>2.992461252661037E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.02992461252661037</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.12347964605337609</v>
+        <v>0.1234796460533761</v>
       </c>
       <c r="C5">
         <v>0.1234796466906095</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.29782338828919219</v>
+        <v>0.2978233882891922</v>
       </c>
       <c r="C6">
-        <v>0.29782337935710068</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2978233793571007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1.0904137530296589E-2</v>
+        <v>0.01090413753029659</v>
       </c>
       <c r="C7">
-        <v>1.0904130156140741E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.01090413015614074</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -559,40 +504,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>4.5143928922989081E-2</v>
+        <v>0.04514392892298908</v>
       </c>
       <c r="C9">
-        <v>4.5143936653585279E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.04514393665358528</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>4.8843318133160438E-2</v>
+        <v>0.04884331813316044</v>
       </c>
       <c r="C10">
-        <v>4.8843310102599381E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.04884331010259938</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>4.5091210520712383E-2</v>
+        <v>0.04509121052071238</v>
       </c>
       <c r="C11">
-        <v>4.5091213616032112E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.04509121361603211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -603,20 +548,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>3.0992543809448578E-2</v>
+        <v>0.03099254380944858</v>
       </c>
       <c r="C13">
-        <v>3.099254015091614E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>14</v>
+        <v>0.03099254015091614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jupyter Notebook that runs
Jupyter Notebook by thte name Basic Plotting (1).ipynb runs and fully funcation as an interactive notebook. I cam commiting this to show that this has worked so far.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.092811143995738e-18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -446,7 +446,7 @@
         <v>0.3677972395916179</v>
       </c>
       <c r="C3">
-        <v>0.3677972307464058</v>
+        <v>0.8422882724052781</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -457,7 +457,7 @@
         <v>0.02992458714920683</v>
       </c>
       <c r="C4">
-        <v>0.02992461252661037</v>
+        <v>3.547663963132689e-05</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -468,7 +468,7 @@
         <v>0.1234796460533761</v>
       </c>
       <c r="C5">
-        <v>0.1234796466906095</v>
+        <v>9.776561004032234e-19</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -479,7 +479,7 @@
         <v>0.2978233882891922</v>
       </c>
       <c r="C6">
-        <v>0.2978233793571007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -490,7 +490,7 @@
         <v>0.01090413753029659</v>
       </c>
       <c r="C7">
-        <v>0.01090413015614074</v>
+        <v>3.642974848100913e-18</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>3.177071318118062e-18</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -512,7 +512,7 @@
         <v>0.04514392892298908</v>
       </c>
       <c r="C9">
-        <v>0.04514393665358528</v>
+        <v>0.00219714938765768</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -523,7 +523,7 @@
         <v>0.04884331813316044</v>
       </c>
       <c r="C10">
-        <v>0.04884331010259938</v>
+        <v>0.006090650936498306</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -534,7 +534,7 @@
         <v>0.04509121052071238</v>
       </c>
       <c r="C11">
-        <v>0.04509121361603211</v>
+        <v>0.0003074966821064281</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>5.283386679673052e-21</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -556,7 +556,7 @@
         <v>0.03099254380944858</v>
       </c>
       <c r="C13">
-        <v>0.03099254015091614</v>
+        <v>0.149080953948828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Current version runs beautifully!
We run on the jupyter notebook called Basic Plotting (1).ipynb the code from the python file vpn_code_that_semi_works.py with all functions i.e. charts, interactiveness etc.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2.092811143995738e-18</v>
+        <v>5.310557155020105e-18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -446,7 +446,7 @@
         <v>0.3677972395916179</v>
       </c>
       <c r="C3">
-        <v>0.8422882724052781</v>
+        <v>0.4223910921055155</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -457,7 +457,7 @@
         <v>0.02992458714920683</v>
       </c>
       <c r="C4">
-        <v>3.547663963132689e-05</v>
+        <v>1.647883696604348e-17</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -468,7 +468,7 @@
         <v>0.1234796460533761</v>
       </c>
       <c r="C5">
-        <v>9.776561004032234e-19</v>
+        <v>2.2026897714741e-17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -479,7 +479,7 @@
         <v>0.2978233882891922</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.3266462031418655</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -490,7 +490,7 @@
         <v>0.01090413753029659</v>
       </c>
       <c r="C7">
-        <v>3.642974848100913e-18</v>
+        <v>8.476572151579813e-19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>3.177071318118062e-18</v>
+        <v>5.424406555728697e-18</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -512,7 +512,7 @@
         <v>0.04514392892298908</v>
       </c>
       <c r="C9">
-        <v>0.00219714938765768</v>
+        <v>0.02173475375986822</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -523,7 +523,7 @@
         <v>0.04884331813316044</v>
       </c>
       <c r="C10">
-        <v>0.006090650936498306</v>
+        <v>1.96004155244827e-18</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -534,7 +534,7 @@
         <v>0.04509121052071238</v>
       </c>
       <c r="C11">
-        <v>0.0003074966821064281</v>
+        <v>6.794645933682366e-18</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>5.283386679673052e-21</v>
+        <v>2.0495369838691e-18</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -556,7 +556,7 @@
         <v>0.03099254380944858</v>
       </c>
       <c r="C13">
-        <v>0.149080953948828</v>
+        <v>0.2292279509927508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chaning what we display to make sure it works perfectly!
You have to run it 3-4 times with the previous code to have it display everything perfectly i.e. charts, interactiveness.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5.310557155020105e-18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -446,7 +446,7 @@
         <v>0.3677972395916179</v>
       </c>
       <c r="C3">
-        <v>0.4223910921055155</v>
+        <v>0.3677972307464058</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -457,7 +457,7 @@
         <v>0.02992458714920683</v>
       </c>
       <c r="C4">
-        <v>1.647883696604348e-17</v>
+        <v>0.02992461252661037</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -468,7 +468,7 @@
         <v>0.1234796460533761</v>
       </c>
       <c r="C5">
-        <v>2.2026897714741e-17</v>
+        <v>0.1234796466906095</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -479,7 +479,7 @@
         <v>0.2978233882891922</v>
       </c>
       <c r="C6">
-        <v>0.3266462031418655</v>
+        <v>0.2978233793571007</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -490,7 +490,7 @@
         <v>0.01090413753029659</v>
       </c>
       <c r="C7">
-        <v>8.476572151579813e-19</v>
+        <v>0.01090413015614074</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>5.424406555728697e-18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -512,7 +512,7 @@
         <v>0.04514392892298908</v>
       </c>
       <c r="C9">
-        <v>0.02173475375986822</v>
+        <v>0.04514393665358528</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -523,7 +523,7 @@
         <v>0.04884331813316044</v>
       </c>
       <c r="C10">
-        <v>1.96004155244827e-18</v>
+        <v>0.04884331010259938</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -534,7 +534,7 @@
         <v>0.04509121052071238</v>
       </c>
       <c r="C11">
-        <v>6.794645933682366e-18</v>
+        <v>0.04509121361603211</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>2.0495369838691e-18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -556,7 +556,7 @@
         <v>0.03099254380944858</v>
       </c>
       <c r="C13">
-        <v>0.2292279509927508</v>
+        <v>0.03099254015091614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed the calling of a function to prevent unnecessary printing
We no longer call function solve_initial_opt_weight() on its own since that return non-useful printing of the frontier etc. in matrices
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.330246048421937e-19</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -446,7 +446,7 @@
         <v>0.3677972395916179</v>
       </c>
       <c r="C3">
-        <v>0.3677972307464058</v>
+        <v>0.4458327234947346</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -457,7 +457,7 @@
         <v>0.02992458714920683</v>
       </c>
       <c r="C4">
-        <v>0.02992461252661037</v>
+        <v>0.06357623681831188</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -468,7 +468,7 @@
         <v>0.1234796460533761</v>
       </c>
       <c r="C5">
-        <v>0.1234796466906095</v>
+        <v>8.807695185509702e-18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -479,7 +479,7 @@
         <v>0.2978233882891922</v>
       </c>
       <c r="C6">
-        <v>0.2978233793571007</v>
+        <v>0.3486403815655779</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -490,7 +490,7 @@
         <v>0.01090413753029659</v>
       </c>
       <c r="C7">
-        <v>0.01090413015614074</v>
+        <v>3.661815218948759e-19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>9.653876486319454e-19</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -512,7 +512,7 @@
         <v>0.04514392892298908</v>
       </c>
       <c r="C9">
-        <v>0.04514393665358528</v>
+        <v>0.05261526521361033</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -523,7 +523,7 @@
         <v>0.04884331813316044</v>
       </c>
       <c r="C10">
-        <v>0.04884331010259938</v>
+        <v>0.02203726983585222</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -534,7 +534,7 @@
         <v>0.04509121052071238</v>
       </c>
       <c r="C11">
-        <v>0.04509121361603211</v>
+        <v>0.05890727244953593</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -556,7 +556,7 @@
         <v>0.03099254380944858</v>
       </c>
       <c r="C13">
-        <v>0.03099254015091614</v>
+        <v>0.008390850622377223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed the upload to cde button
We removed an unnecessary button that was called "Upload to CDE" by commenting it out.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2.330246048421937e-19</v>
+        <v>0.1049893408696204</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -446,7 +446,7 @@
         <v>0.3677972395916179</v>
       </c>
       <c r="C3">
-        <v>0.4458327234947346</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -457,7 +457,7 @@
         <v>0.02992458714920683</v>
       </c>
       <c r="C4">
-        <v>0.06357623681831188</v>
+        <v>0.1618706169496776</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -468,7 +468,7 @@
         <v>0.1234796460533761</v>
       </c>
       <c r="C5">
-        <v>8.807695185509702e-18</v>
+        <v>3.582521641092274e-17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -479,7 +479,7 @@
         <v>0.2978233882891922</v>
       </c>
       <c r="C6">
-        <v>0.3486403815655779</v>
+        <v>0.7325499012809557</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -490,7 +490,7 @@
         <v>0.01090413753029659</v>
       </c>
       <c r="C7">
-        <v>3.661815218948759e-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>9.653876486319454e-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -512,7 +512,7 @@
         <v>0.04514392892298908</v>
       </c>
       <c r="C9">
-        <v>0.05261526521361033</v>
+        <v>0.0004661450251538002</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -523,7 +523,7 @@
         <v>0.04884331813316044</v>
       </c>
       <c r="C10">
-        <v>0.02203726983585222</v>
+        <v>4.155213597677616e-17</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -534,7 +534,7 @@
         <v>0.04509121052071238</v>
       </c>
       <c r="C11">
-        <v>0.05890727244953593</v>
+        <v>0.0001239958745925973</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>2.788770720769446e-18</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -556,7 +556,7 @@
         <v>0.03099254380944858</v>
       </c>
       <c r="C13">
-        <v>0.008390850622377223</v>
+        <v>1.958378521762924e-18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the display of additional and unnecessary sliders
We commented out a line that forcefully displayed sliders. This line was left in from previous attempts to have sliders dislayed that were not successful due to the wrong implementation of bqplot. As a result, now that the rest of the interactive bqplot requiring items are displayed the ended up displaying additional and unwanted sliders.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.1049893408696204</v>
+        <v>5.346288662278841e-20</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -443,10 +443,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.3677972395916179</v>
+        <v>0.4250667495367802</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.3698035559332329</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -454,10 +454,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.02992458714920683</v>
+        <v>0.02283686003961818</v>
       </c>
       <c r="C4">
-        <v>0.1618706169496776</v>
+        <v>2.719181816842377e-18</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -465,10 +465,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.1234796460533761</v>
+        <v>2.059984127722458e-17</v>
       </c>
       <c r="C5">
-        <v>3.582521641092274e-17</v>
+        <v>4.683478700650488e-17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -476,10 +476,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.2978233882891922</v>
+        <v>0.3260486671197617</v>
       </c>
       <c r="C6">
-        <v>0.7325499012809557</v>
+        <v>0.3176571920514362</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -487,10 +487,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.01090413753029659</v>
+        <v>1.965116437629977e-18</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.01762138445562067</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -498,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2.727446090158847e-19</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -509,10 +509,10 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.04514392892298908</v>
+        <v>0.03395846391654626</v>
       </c>
       <c r="C9">
-        <v>0.0004661450251538002</v>
+        <v>0.05108086275464575</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -520,10 +520,10 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.04884331813316044</v>
+        <v>0.03464765278391641</v>
       </c>
       <c r="C10">
-        <v>4.155213597677616e-17</v>
+        <v>0.07663993609146461</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -531,10 +531,10 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.04509121052071238</v>
+        <v>0.09670723458172271</v>
       </c>
       <c r="C11">
-        <v>0.0001239958745925973</v>
+        <v>3.993166304001589e-18</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>2.788770720769446e-18</v>
+        <v>1.492601215055902e-17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -553,10 +553,10 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.03099254380944858</v>
+        <v>0.0607343720216545</v>
       </c>
       <c r="C13">
-        <v>1.958378521762924e-18</v>
+        <v>0.1671970687136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Works with Apolis fund
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Opt Portfolio</t>
   </si>
@@ -22,40 +22,55 @@
     <t>Opt Portfolio with View</t>
   </si>
   <si>
-    <t>Emerging Mkts</t>
-  </si>
-  <si>
-    <t>US Treasuries</t>
-  </si>
-  <si>
-    <t>High Yield</t>
-  </si>
-  <si>
-    <t>Int'l Bonds</t>
-  </si>
-  <si>
-    <t>Bonds - Agg</t>
-  </si>
-  <si>
-    <t>Russ 1K Gro</t>
-  </si>
-  <si>
-    <t>GOLD</t>
-  </si>
-  <si>
-    <t>Commodities</t>
-  </si>
-  <si>
-    <t>Small Stocks</t>
-  </si>
-  <si>
-    <t>Russ 1K Val</t>
-  </si>
-  <si>
-    <t>Real Estate</t>
-  </si>
-  <si>
-    <t>S&amp;P 500</t>
+    <t>US High Yield Bonds</t>
+  </si>
+  <si>
+    <t>US Equity</t>
+  </si>
+  <si>
+    <t>Spanish Equity</t>
+  </si>
+  <si>
+    <t>MSCI World</t>
+  </si>
+  <si>
+    <t>MSCI Info tech</t>
+  </si>
+  <si>
+    <t>Italian Equity</t>
+  </si>
+  <si>
+    <t>Greek Govies</t>
+  </si>
+  <si>
+    <t>Greek Equity</t>
+  </si>
+  <si>
+    <t>German Equity</t>
+  </si>
+  <si>
+    <t>European Equity</t>
+  </si>
+  <si>
+    <t>European Corp</t>
+  </si>
+  <si>
+    <t>European Banks</t>
+  </si>
+  <si>
+    <t>EU High Yield Bonds</t>
+  </si>
+  <si>
+    <t>Emerging Asia Equity</t>
+  </si>
+  <si>
+    <t>Chinese Equity</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>1-5 years GILTS</t>
   </si>
 </sst>
 </file>
@@ -413,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,10 +447,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.00315492070843431</v>
       </c>
       <c r="C2">
-        <v>3.885780586188048e-16</v>
+        <v>0.003154966570271506</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -443,10 +458,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>9.783840404509192e-16</v>
+        <v>0.004199034084009822</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.004199030326780291</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -454,10 +469,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.0003611873133961651</v>
       </c>
       <c r="C4">
-        <v>6.245004513516506e-16</v>
+        <v>0.0003611815471370783</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -465,10 +480,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.003819085444500003</v>
       </c>
       <c r="C5">
-        <v>1.02695629777827e-15</v>
+        <v>0.003819095342884271</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -476,10 +491,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.003935802368980387</v>
       </c>
       <c r="C6">
-        <v>2.498001805406602e-16</v>
+        <v>0.003935797963162609</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -487,10 +502,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.005193523401558717</v>
       </c>
       <c r="C7">
-        <v>1.006139616066548e-15</v>
+        <v>0.00519350476374041</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -498,10 +513,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1.501718098835149e-05</v>
       </c>
       <c r="C8">
-        <v>4.305366826939938e-16</v>
+        <v>1.501248085167256e-05</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -509,7 +524,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>5.412337245047638e-16</v>
+        <v>3.941484905584094e-21</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -520,10 +535,10 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>2.359223927328458e-16</v>
+        <v>0.009319271088750667</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.009319274914133967</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -531,10 +546,10 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.005819668809611802</v>
       </c>
       <c r="C11">
-        <v>4.024558464266192e-16</v>
+        <v>0.005819676705408487</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -542,10 +557,10 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.1953501833099527</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.1953501607042582</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -553,10 +568,65 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0.01453939738842425</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.01453939117218285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.002389090340788871</v>
+      </c>
+      <c r="C14">
+        <v>0.002389111646993501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.0002622190250429839</v>
+      </c>
+      <c r="C15">
+        <v>0.0002622059321314265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.006044244303905958</v>
+      </c>
+      <c r="C16">
+        <v>0.006044254311253346</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>0.370532592559188</v>
+      </c>
+      <c r="C17">
+        <v>0.370532570333677</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>0.3750647626724672</v>
+      </c>
+      <c r="C18">
+        <v>0.3750647652851333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code now works with Apolis Fund products
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Opt Portfolio</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Chinese Equity</t>
-  </si>
-  <si>
-    <t>Cash</t>
   </si>
   <si>
     <t>1-5 years GILTS</t>
@@ -428,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,10 +444,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.00315492070843431</v>
+        <v>0.02998349699801747</v>
       </c>
       <c r="C2">
-        <v>0.003154966570271506</v>
+        <v>0.02997980578320772</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -458,10 +455,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.004199034084009822</v>
+        <v>1.761589625444573e-19</v>
       </c>
       <c r="C3">
-        <v>0.004199030326780291</v>
+        <v>3.862800410783512e-19</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -469,10 +466,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.0003611873133961651</v>
+        <v>1.761589625444573e-19</v>
       </c>
       <c r="C4">
-        <v>0.0003611815471370783</v>
+        <v>1.62748231801186e-19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -480,10 +477,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.003819085444500003</v>
+        <v>2.439454888092385e-19</v>
       </c>
       <c r="C5">
-        <v>0.003819095342884271</v>
+        <v>1.62748231801186e-19</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -491,10 +488,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.003935802368980387</v>
+        <v>2.752045353098075e-19</v>
       </c>
       <c r="C6">
-        <v>0.003935797963162609</v>
+        <v>2.846691045382254e-19</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -502,10 +499,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.005193523401558717</v>
+        <v>0.002899558148691509</v>
       </c>
       <c r="C7">
-        <v>0.00519350476374041</v>
+        <v>0.002899779144328617</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -513,10 +510,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>1.501718098835149e-05</v>
+        <v>0.0219351662951515</v>
       </c>
       <c r="C8">
-        <v>1.501248085167256e-05</v>
+        <v>0.0219363217695006</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -524,10 +521,10 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>3.941484905584094e-21</v>
+        <v>0.03294249137981119</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.0329428682566893</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -535,10 +532,10 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.009319271088750667</v>
+        <v>8.806444213787078e-20</v>
       </c>
       <c r="C10">
-        <v>0.009319274914133967</v>
+        <v>1.423345522691127e-19</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -546,10 +543,10 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.005819668809611802</v>
+        <v>0.002411575005719938</v>
       </c>
       <c r="C11">
-        <v>0.005819676705408487</v>
+        <v>0.002411783866887989</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -557,10 +554,10 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.1953501833099527</v>
+        <v>0.6949378640760929</v>
       </c>
       <c r="C12">
-        <v>0.1953501607042582</v>
+        <v>0.6949474739127106</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -568,10 +565,10 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.01453939738842425</v>
+        <v>0.0008727300330695211</v>
       </c>
       <c r="C13">
-        <v>0.01453939117218285</v>
+        <v>0.0008727562585592101</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -579,10 +576,10 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.002389090340788871</v>
+        <v>0.05277490247116246</v>
       </c>
       <c r="C14">
-        <v>0.002389111646993501</v>
+        <v>0.05277251263754121</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -590,10 +587,10 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.0002622190250429839</v>
+        <v>3.247273216924826e-19</v>
       </c>
       <c r="C15">
-        <v>0.0002622059321314265</v>
+        <v>4.95220678144552e-20</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -601,10 +598,10 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.006044244303905958</v>
+        <v>0.01684847136174504</v>
       </c>
       <c r="C16">
-        <v>0.006044254311253346</v>
+        <v>0.01684995209365592</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -612,21 +609,10 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.370532592559188</v>
+        <v>0.1443937442305386</v>
       </c>
       <c r="C17">
-        <v>0.370532570333677</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>0.3750647626724672</v>
-      </c>
-      <c r="C18">
-        <v>0.3750647652851333</v>
+        <v>0.1443867462769187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding explanatory comments to our code.
We add additional comments to the code.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -447,7 +447,7 @@
         <v>0.02998349699801747</v>
       </c>
       <c r="C2">
-        <v>0.02997980578320772</v>
+        <v>3.416580644237559e-18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -458,7 +458,7 @@
         <v>1.761589625444573e-19</v>
       </c>
       <c r="C3">
-        <v>3.862800410783512e-19</v>
+        <v>1.256525404968262e-17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -469,7 +469,7 @@
         <v>1.761589625444573e-19</v>
       </c>
       <c r="C4">
-        <v>1.62748231801186e-19</v>
+        <v>6.423044353443471e-18</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -480,7 +480,7 @@
         <v>2.439454888092385e-19</v>
       </c>
       <c r="C5">
-        <v>1.62748231801186e-19</v>
+        <v>5.608016481145033e-19</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -491,7 +491,7 @@
         <v>2.752045353098075e-19</v>
       </c>
       <c r="C6">
-        <v>2.846691045382254e-19</v>
+        <v>4.105796903885244e-18</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -502,7 +502,7 @@
         <v>0.002899558148691509</v>
       </c>
       <c r="C7">
-        <v>0.002899779144328617</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -513,7 +513,7 @@
         <v>0.0219351662951515</v>
       </c>
       <c r="C8">
-        <v>0.0219363217695006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -524,7 +524,7 @@
         <v>0.03294249137981119</v>
       </c>
       <c r="C9">
-        <v>0.0329428682566893</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -535,7 +535,7 @@
         <v>8.806444213787078e-20</v>
       </c>
       <c r="C10">
-        <v>1.423345522691127e-19</v>
+        <v>1.212151697752774e-18</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -546,7 +546,7 @@
         <v>0.002411575005719938</v>
       </c>
       <c r="C11">
-        <v>0.002411783866887989</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -557,7 +557,7 @@
         <v>0.6949378640760929</v>
       </c>
       <c r="C12">
-        <v>0.6949474739127106</v>
+        <v>3.158883754877052e-18</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -568,7 +568,7 @@
         <v>0.0008727300330695211</v>
       </c>
       <c r="C13">
-        <v>0.0008727562585592101</v>
+        <v>9.755461367149147e-18</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -579,7 +579,7 @@
         <v>0.05277490247116246</v>
       </c>
       <c r="C14">
-        <v>0.05277251263754121</v>
+        <v>0.5775361384257475</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -590,7 +590,7 @@
         <v>3.247273216924826e-19</v>
       </c>
       <c r="C15">
-        <v>4.95220678144552e-20</v>
+        <v>7.635978195447155e-18</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -601,7 +601,7 @@
         <v>0.01684847136174504</v>
       </c>
       <c r="C16">
-        <v>0.01684995209365592</v>
+        <v>4.694572097135503e-18</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -612,7 +612,7 @@
         <v>0.1443937442305386</v>
       </c>
       <c r="C17">
-        <v>0.1443867462769187</v>
+        <v>0.4224638615742526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The code is running very well and as expected in this current configuration.
When run the code will output good and logical results. It assigns the majority of the portfolio to sure and stable assets such as bonds. If the return of those is then taken to negative territory with the slider controlling the views, the new Black Litterman weights will respond logically and assign practically zero portion of the portfolio to those assets.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -447,7 +447,7 @@
         <v>0.02998349699801747</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.2466370749492557</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -458,7 +458,7 @@
         <v>1.761589625444573e-19</v>
       </c>
       <c r="C3">
-        <v>3.260804054269001e-20</v>
+        <v>0.009846537327280743</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -469,7 +469,7 @@
         <v>1.761589625444573e-19</v>
       </c>
       <c r="C4">
-        <v>9.081217886667661e-19</v>
+        <v>0.00072850246583498</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -480,7 +480,7 @@
         <v>2.439454888092385e-19</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.02816842647723668</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -491,7 +491,7 @@
         <v>2.752045353098075e-19</v>
       </c>
       <c r="C6">
-        <v>3.457218936750106e-18</v>
+        <v>1.708316993799091e-18</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -502,7 +502,7 @@
         <v>0.002899558148691509</v>
       </c>
       <c r="C7">
-        <v>2.827077658597984e-18</v>
+        <v>0.000774521279597736</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -513,7 +513,7 @@
         <v>0.0219351662951515</v>
       </c>
       <c r="C8">
-        <v>2.827077658597984e-18</v>
+        <v>0.02311043898291583</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -524,7 +524,7 @@
         <v>0.03294249137981119</v>
       </c>
       <c r="C9">
-        <v>0.03302508923960513</v>
+        <v>0.1101516327223209</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -535,7 +535,7 @@
         <v>8.806444213787078e-20</v>
       </c>
       <c r="C10">
-        <v>1.6304020271345e-20</v>
+        <v>0.0002008355530203714</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -546,7 +546,7 @@
         <v>0.002411575005719938</v>
       </c>
       <c r="C11">
-        <v>8.152010135672502e-21</v>
+        <v>0.02204372345666923</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -557,7 +557,7 @@
         <v>0.6949378640760929</v>
       </c>
       <c r="C12">
-        <v>0.6996651823201925</v>
+        <v>3.01153745330273e-17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -568,7 +568,7 @@
         <v>0.0008727300330695211</v>
       </c>
       <c r="C13">
-        <v>2.225468415920716e-18</v>
+        <v>7.692741145799391e-05</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -579,7 +579,7 @@
         <v>0.05277490247116246</v>
       </c>
       <c r="C14">
-        <v>0.01357995565580946</v>
+        <v>0.326582795141821</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -590,7 +590,7 @@
         <v>3.247273216924826e-19</v>
       </c>
       <c r="C15">
-        <v>3.243516722644059e-17</v>
+        <v>0.0002056051372634622</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -601,7 +601,7 @@
         <v>0.01684847136174504</v>
       </c>
       <c r="C16">
-        <v>0.06376851999281302</v>
+        <v>0.01974258369999374</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -612,7 +612,7 @@
         <v>0.1443937442305386</v>
       </c>
       <c r="C17">
-        <v>0.1899612527915799</v>
+        <v>0.2117303953953317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Applied new input to the code.
In this version we supply as input to our code a new data file, originally called "TEA-...". We also re-arrange our input files away from the Main folder into the archive folder to avoid cluttering of our main workspace. We created a new data folder called "Cleaned" which will contani our data in cleaned form such that we can then simply copy the file that we want to the "Main" directory, rename it to "prices" (which is the input for which our code looks) and then simply run it.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Opt Portfolio</t>
   </si>
@@ -22,52 +22,25 @@
     <t>Opt Portfolio with View</t>
   </si>
   <si>
-    <t>US High Yield Bonds</t>
-  </si>
-  <si>
-    <t>US Equity</t>
-  </si>
-  <si>
-    <t>Spanish Equity</t>
-  </si>
-  <si>
-    <t>MSCI World</t>
-  </si>
-  <si>
-    <t>MSCI Info tech</t>
-  </si>
-  <si>
-    <t>Italian Equity</t>
-  </si>
-  <si>
-    <t>Greek Govies</t>
-  </si>
-  <si>
-    <t>Greek Equity</t>
-  </si>
-  <si>
-    <t>German Equity</t>
-  </si>
-  <si>
-    <t>European Equity</t>
-  </si>
-  <si>
-    <t>European Corp</t>
-  </si>
-  <si>
-    <t>European Banks</t>
-  </si>
-  <si>
-    <t>EU High Yield Bonds</t>
-  </si>
-  <si>
-    <t>Emerging Asia Equity</t>
-  </si>
-  <si>
-    <t>Chinese Equity</t>
-  </si>
-  <si>
-    <t>1-5 years GILTS</t>
+    <t>EUR001M Index</t>
+  </si>
+  <si>
+    <t>LEF1TREU Index</t>
+  </si>
+  <si>
+    <t>SX5R Index</t>
+  </si>
+  <si>
+    <t>SXUSR Index	US</t>
+  </si>
+  <si>
+    <t>BEGCGA Index</t>
+  </si>
+  <si>
+    <t>LEC4TREU Index</t>
+  </si>
+  <si>
+    <t>LEATTREU Index</t>
   </si>
 </sst>
 </file>
@@ -425,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,10 +417,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.02998349699801747</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.2466370749492557</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -455,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1.761589625444573e-19</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.009846537327280743</v>
+        <v>3.05311331771918e-16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -466,10 +439,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1.761589625444573e-19</v>
+        <v>6.436803831546e-16</v>
       </c>
       <c r="C4">
-        <v>0.00072850246583498</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -477,10 +450,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2.439454888092385e-19</v>
+        <v>3.787206496253191e-16</v>
       </c>
       <c r="C5">
-        <v>0.02816842647723668</v>
+        <v>3.200284730239067e-17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -488,10 +461,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>2.752045353098075e-19</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1.708316993799091e-18</v>
+        <v>5.560422236538279e-16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -499,10 +472,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.002899558148691509</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>0.000774521279597736</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -510,109 +483,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.0219351662951515</v>
+        <v>2.517749162550946e-15</v>
       </c>
       <c r="C8">
-        <v>0.02311043898291583</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>0.03294249137981119</v>
-      </c>
-      <c r="C9">
-        <v>0.1101516327223209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>8.806444213787078e-20</v>
-      </c>
-      <c r="C10">
-        <v>0.0002008355530203714</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>0.002411575005719938</v>
-      </c>
-      <c r="C11">
-        <v>0.02204372345666923</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>0.6949378640760929</v>
-      </c>
-      <c r="C12">
-        <v>3.01153745330273e-17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>0.0008727300330695211</v>
-      </c>
-      <c r="C13">
-        <v>7.692741145799391e-05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.05277490247116246</v>
-      </c>
-      <c r="C14">
-        <v>0.326582795141821</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>3.247273216924826e-19</v>
-      </c>
-      <c r="C15">
-        <v>0.0002056051372634622</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0.01684847136174504</v>
-      </c>
-      <c r="C16">
-        <v>0.01974258369999374</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>0.1443937442305386</v>
-      </c>
-      <c r="C17">
-        <v>0.2117303953953317</v>
+        <v>1.206421473722328e-15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running the model with Cash
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -22,25 +22,25 @@
     <t>Opt Portfolio with View</t>
   </si>
   <si>
-    <t>EUR001M Index</t>
-  </si>
-  <si>
-    <t>LEF1TREU Index</t>
-  </si>
-  <si>
-    <t>SX5R Index</t>
-  </si>
-  <si>
-    <t>SXUSR Index	US</t>
-  </si>
-  <si>
-    <t>BEGCGA Index</t>
-  </si>
-  <si>
-    <t>LEC4TREU Index</t>
-  </si>
-  <si>
-    <t>LEATTREU Index</t>
+    <t>PARSTEI LX Equity</t>
+  </si>
+  <si>
+    <t>FLOT FP Equity</t>
+  </si>
+  <si>
+    <t>SX5EEX GY Equity</t>
+  </si>
+  <si>
+    <t>SPY US Equity</t>
+  </si>
+  <si>
+    <t>LFGGBDR LX Equity</t>
+  </si>
+  <si>
+    <t>EUN5 GY Equity</t>
+  </si>
+  <si>
+    <t>EUNH GY Equity</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.9999999999999998</v>
+        <v>0.9999999999999986</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -431,7 +431,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>3.05311331771918e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -439,10 +439,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>6.436803831546e-16</v>
+        <v>5.415120407071345e-16</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>8.292679237873184e-16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -450,10 +450,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>3.787206496253191e-16</v>
+        <v>4.567492532905971e-16</v>
       </c>
       <c r="C5">
-        <v>3.200284730239067e-17</v>
+        <v>6.684234565806446e-16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -461,10 +461,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>8.981681503671817e-16</v>
       </c>
       <c r="C6">
-        <v>5.560422236538279e-16</v>
+        <v>1.077585560291168e-15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>9.204482471635608e-16</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -483,10 +483,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>2.517749162550946e-15</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1.206421473722328e-15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Runs with sensible Weights.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -417,10 +417,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.3921459680713356</v>
       </c>
       <c r="C2">
-        <v>0.9999999999999986</v>
+        <v>0.4690580135690283</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -428,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.1938669551675961</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.1186057994486912</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -439,10 +439,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>5.415120407071345e-16</v>
+        <v>0.0677949822057861</v>
       </c>
       <c r="C4">
-        <v>8.292679237873184e-16</v>
+        <v>0.06717876075738202</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -450,10 +450,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>4.567492532905971e-16</v>
+        <v>0.06719666705145336</v>
       </c>
       <c r="C5">
-        <v>6.684234565806446e-16</v>
+        <v>0.0671787607573822</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -461,10 +461,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>8.981681503671817e-16</v>
+        <v>0.07195801386525061</v>
       </c>
       <c r="C6">
-        <v>1.077585560291168e-15</v>
+        <v>0.06717876075738212</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -472,10 +472,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.08419062385962513</v>
       </c>
       <c r="C7">
-        <v>9.204482471635608e-16</v>
+        <v>0.08023122541279935</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -483,10 +483,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.1228467897789531</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.130568679297338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Indicating the Location of the Return Target we set
We set a lower bound to the return that we require the portfolio to provide.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -417,10 +417,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.3921459680713356</v>
+        <v>0.2685990624464732</v>
       </c>
       <c r="C2">
-        <v>0.4690580135690283</v>
+        <v>0.2685990624464732</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -428,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.1938669551675961</v>
+        <v>0.2595668476817547</v>
       </c>
       <c r="C3">
-        <v>0.1186057994486912</v>
+        <v>0.2595668476817547</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -439,10 +439,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.0677949822057861</v>
+        <v>8.673617379884035e-19</v>
       </c>
       <c r="C4">
-        <v>0.06717876075738202</v>
+        <v>8.673617379884035e-19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -450,10 +450,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.06719666705145336</v>
+        <v>3.035766082959412e-18</v>
       </c>
       <c r="C5">
-        <v>0.0671787607573822</v>
+        <v>3.035766082959412e-18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -461,10 +461,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.07195801386525061</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0.06717876075738212</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -472,10 +472,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.08419062385962513</v>
+        <v>0.2410965409232599</v>
       </c>
       <c r="C7">
-        <v>0.08023122541279935</v>
+        <v>0.2410965409232599</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -483,10 +483,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.1228467897789531</v>
+        <v>0.2307375489485121</v>
       </c>
       <c r="C8">
-        <v>0.130568679297338</v>
+        <v>0.2307375489485121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Understood the workings of the float slider
To type in a value you are required to type the value you like by dividing it in your mind by 100. Meaning that if you want to input a "view" of 5% you need to type in 0.05. I would like to search where exactly the values are read in and then divide those by 100 so that the user will be able to input 5 and the code to understand 0.05 in reality
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -417,10 +417,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.2685990624464732</v>
+        <v>0.2454406141024289</v>
       </c>
       <c r="C2">
-        <v>0.2685990624464732</v>
+        <v>0.245440628078421</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -428,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.2595668476817547</v>
+        <v>0.1815773618901335</v>
       </c>
       <c r="C3">
-        <v>0.2595668476817547</v>
+        <v>0.1815773450933061</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -439,10 +439,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>8.673617379884035e-19</v>
+        <v>0.09883777827451906</v>
       </c>
       <c r="C4">
-        <v>8.673617379884035e-19</v>
+        <v>0.09883777827451899</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -450,10 +450,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>3.035766082959412e-18</v>
+        <v>0.09883777827451906</v>
       </c>
       <c r="C5">
-        <v>3.035766082959412e-18</v>
+        <v>0.09883777827451901</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -461,10 +461,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.09883777827451906</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.09883777827451899</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -472,10 +472,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.2410965409232599</v>
+        <v>0.11995695347692</v>
       </c>
       <c r="C7">
-        <v>0.2410965409232599</v>
+        <v>0.1199569551788409</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -483,10 +483,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.2307375489485121</v>
+        <v>0.1565117357069661</v>
       </c>
       <c r="C8">
-        <v>0.2307375489485121</v>
+        <v>0.1565117368258783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Currently works with 3 bars
One bar is Initial Weights then second is Mkt Efficient Portfolio and final is Efficient Portfolio with Views
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Initial Weights</t>
+  </si>
   <si>
     <t>Opt Portfolio</t>
   </si>
@@ -398,94 +401,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
         <v>0.2454406141024289</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.245440628078421</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
+        <v>0.05</v>
+      </c>
+      <c r="C3">
         <v>0.1815773618901335</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.1815773450933061</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4">
         <v>0.09883777827451906</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.09883777827451899</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
         <v>0.09883777827451906</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.09883777827451901</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6">
+        <v>0.15</v>
+      </c>
+      <c r="C6">
         <v>0.09883777827451906</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.09883777827451899</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7">
+        <v>0.2</v>
+      </c>
+      <c r="C7">
         <v>0.11995695347692</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.1199569551788409</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
+        <v>0.3</v>
+      </c>
+      <c r="C8">
         <v>0.1565117357069661</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.1565117368258783</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changing the Risk-free rate
We changed the risk free rate to zero to reflect current economic conditions. The initial risk-free rate was set by the US team developing this code where the economic enviroment reflected such an estimation. On the contrary in the EU with the pandemic environment  we need to lower it significantly down to zero.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.2454406141024289</v>
+        <v>0.562341192568151</v>
       </c>
       <c r="D2">
-        <v>0.245440628078421</v>
+        <v>0.562341192568151</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.1815773618901335</v>
+        <v>0.3584989408622693</v>
       </c>
       <c r="D3">
-        <v>0.1815773450933061</v>
+        <v>0.3584989408622693</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,10 +454,10 @@
         <v>0.1</v>
       </c>
       <c r="C4">
-        <v>0.09883777827451906</v>
+        <v>4.336808689942018e-19</v>
       </c>
       <c r="D4">
-        <v>0.09883777827451899</v>
+        <v>4.336808689942018e-19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.09883777827451906</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.09883777827451901</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +482,10 @@
         <v>0.15</v>
       </c>
       <c r="C6">
-        <v>0.09883777827451906</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0.09883777827451899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.11995695347692</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.1199569551788409</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,10 +510,10 @@
         <v>0.3</v>
       </c>
       <c r="C8">
-        <v>0.1565117357069661</v>
+        <v>0.07915986656957973</v>
       </c>
       <c r="D8">
-        <v>0.1565117368258783</v>
+        <v>0.07915986656957973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Archiving the latest input file uploaded by ayfado
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.562341192568151</v>
+        <v>0.2718729031447604</v>
       </c>
       <c r="D2">
-        <v>0.562341192568151</v>
+        <v>0.2718729031447604</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.3584989408622693</v>
+        <v>0.2619866744857898</v>
       </c>
       <c r="D3">
-        <v>0.3584989408622693</v>
+        <v>0.2619866744857898</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,10 +454,10 @@
         <v>0.1</v>
       </c>
       <c r="C4">
-        <v>4.336808689942018e-19</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>4.336808689942018e-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2.846030702774449e-19</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2.846030702774449e-19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +482,10 @@
         <v>0.15</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3.469446951953614e-18</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>3.469446951953614e-18</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.2407114716596564</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.2407114716596564</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,10 +510,10 @@
         <v>0.3</v>
       </c>
       <c r="C8">
-        <v>0.07915986656957973</v>
+        <v>0.2254289507097933</v>
       </c>
       <c r="D8">
-        <v>0.07915986656957973</v>
+        <v>0.2254289507097933</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manually reverting back to previous working commit
The current master commit does not function properly. The responsiveness of the graph does no longer seem to function properly. Hence, we decided to revert back to the previous working commit.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.2718729031447604</v>
+        <v>0.2454406141024289</v>
       </c>
       <c r="D2">
-        <v>0.2718729031447604</v>
+        <v>0.245440628078421</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.2619866744857898</v>
+        <v>0.1815773618901335</v>
       </c>
       <c r="D3">
-        <v>0.2619866744857898</v>
+        <v>0.1815773450933061</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,10 +454,10 @@
         <v>0.1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.09883777827451906</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.09883777827451899</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>2.846030702774449e-19</v>
+        <v>0.09883777827451906</v>
       </c>
       <c r="D5">
-        <v>2.846030702774449e-19</v>
+        <v>0.09883777827451901</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +482,10 @@
         <v>0.15</v>
       </c>
       <c r="C6">
-        <v>3.469446951953614e-18</v>
+        <v>0.09883777827451906</v>
       </c>
       <c r="D6">
-        <v>3.469446951953614e-18</v>
+        <v>0.09883777827451899</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.2407114716596564</v>
+        <v>0.11995695347692</v>
       </c>
       <c r="D7">
-        <v>0.2407114716596564</v>
+        <v>0.1199569551788409</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,10 +510,10 @@
         <v>0.3</v>
       </c>
       <c r="C8">
-        <v>0.2254289507097933</v>
+        <v>0.1565117357069661</v>
       </c>
       <c r="D8">
-        <v>0.2254289507097933</v>
+        <v>0.1565117368258783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reporting Commit: Problem located
Problem was found to be the changing of the risk-free rate. By reducing the risk-free rate to zero the portfolio is then unable to reach the return target of 4% that we have set. As a result, the program breaks down leading to a wrong and unresponsive graph in the end.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.2454406141024289</v>
+        <v>0.1657811205202583</v>
       </c>
       <c r="D2">
-        <v>0.245440628078421</v>
+        <v>0.1657810991108276</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.1815773618901335</v>
+        <v>0.1615951055592954</v>
       </c>
       <c r="D3">
-        <v>0.1815773450933061</v>
+        <v>0.1615950709247715</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,10 +454,10 @@
         <v>0.1</v>
       </c>
       <c r="C4">
-        <v>0.09883777827451906</v>
+        <v>0.124265581389829</v>
       </c>
       <c r="D4">
-        <v>0.09883777827451899</v>
+        <v>0.1242655813898289</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.09883777827451906</v>
+        <v>0.124265581389829</v>
       </c>
       <c r="D5">
-        <v>0.09883777827451901</v>
+        <v>0.124265581389829</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +482,10 @@
         <v>0.15</v>
       </c>
       <c r="C6">
-        <v>0.09883777827451906</v>
+        <v>0.124265581389829</v>
       </c>
       <c r="D6">
-        <v>0.09883777827451899</v>
+        <v>0.124265581389829</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.11995695347692</v>
+        <v>0.1525293361577476</v>
       </c>
       <c r="D7">
-        <v>0.1199569551788409</v>
+        <v>0.1525293532280509</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,10 +510,10 @@
         <v>0.3</v>
       </c>
       <c r="C8">
-        <v>0.1565117357069661</v>
+        <v>0.1472976935932118</v>
       </c>
       <c r="D8">
-        <v>0.1565117368258783</v>
+        <v>0.1472977325668632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solution for previous problem.
As explained in the previous commit we got an unresponsive graph due to a problem in the code. Namely, by reducing the risk free rate down to zero to reflect the current economic environment our portfolio was then unable to reach the 4% target for the return. By reducing the return target down to 1% the portfolio is now able to reach that target and hence the code does not collapse resulting in a responsive graph, as expected.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.1657811205202583</v>
+        <v>0.1559305616838552</v>
       </c>
       <c r="D2">
-        <v>0.1657810991108276</v>
+        <v>0.1559304748967024</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.1615951055592954</v>
+        <v>0.1637229051272682</v>
       </c>
       <c r="D3">
-        <v>0.1615950709247715</v>
+        <v>0.1637228384233602</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,10 +454,10 @@
         <v>0.1</v>
       </c>
       <c r="C4">
-        <v>0.124265581389829</v>
+        <v>0.08546269601881656</v>
       </c>
       <c r="D4">
-        <v>0.1242655813898289</v>
+        <v>0.0854627095093803</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.124265581389829</v>
+        <v>0.07238432245797</v>
       </c>
       <c r="D5">
-        <v>0.124265581389829</v>
+        <v>0.07238423279098104</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +482,10 @@
         <v>0.15</v>
       </c>
       <c r="C6">
-        <v>0.124265581389829</v>
+        <v>0.130098276253158</v>
       </c>
       <c r="D6">
-        <v>0.124265581389829</v>
+        <v>0.130098355694125</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.1525293361577476</v>
+        <v>0.1839516980365401</v>
       </c>
       <c r="D7">
-        <v>0.1525293532280509</v>
+        <v>0.1839517227747055</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,10 +510,10 @@
         <v>0.3</v>
       </c>
       <c r="C8">
-        <v>0.1472976935932118</v>
+        <v>0.208449540422392</v>
       </c>
       <c r="D8">
-        <v>0.1472977325668632</v>
+        <v>0.2084496659107455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Increasing the return target to 2%
We previously lowered the return target to 1% to restore functionality in the code. Now we have increased it up to 3% to reflect more pragmatic results.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.1559305616838552</v>
+        <v>3.876022766635678e-18</v>
       </c>
       <c r="D2">
-        <v>0.1559304748967024</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.1637229051272682</v>
+        <v>0.02124815174069435</v>
       </c>
       <c r="D3">
-        <v>0.1637228384233602</v>
+        <v>0.02124764584718219</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,10 +454,10 @@
         <v>0.1</v>
       </c>
       <c r="C4">
-        <v>0.08546269601881656</v>
+        <v>0.1273388301359862</v>
       </c>
       <c r="D4">
-        <v>0.0854627095093803</v>
+        <v>0.1273383454430054</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.07238432245797</v>
+        <v>0.1697700754744735</v>
       </c>
       <c r="D5">
-        <v>0.07238423279098104</v>
+        <v>0.1697703529919921</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +482,10 @@
         <v>0.15</v>
       </c>
       <c r="C6">
-        <v>0.130098276253158</v>
+        <v>0.2390017860881791</v>
       </c>
       <c r="D6">
-        <v>0.130098355694125</v>
+        <v>0.2390020959213678</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.1839516980365401</v>
+        <v>0.09744088543812593</v>
       </c>
       <c r="D7">
-        <v>0.1839517227747055</v>
+        <v>0.09744157541012331</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,10 +510,10 @@
         <v>0.3</v>
       </c>
       <c r="C8">
-        <v>0.208449540422392</v>
+        <v>0.345200271122541</v>
       </c>
       <c r="D8">
-        <v>0.2084496659107455</v>
+        <v>0.3451999843863293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data labels printed correctly next to bar
We have fixed the issue of printing the data labels in their correct location at the end of the bars of the bar chart.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -423,7 +423,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="C2">
         <v>3.876022766635678e-18</v>
@@ -437,7 +437,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="C3">
         <v>0.02124815174069435</v>
@@ -451,7 +451,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C4">
         <v>0.1273388301359862</v>
@@ -479,7 +479,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C6">
         <v>0.2390017860881791</v>
@@ -493,7 +493,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="C7">
         <v>0.09744088543812593</v>
@@ -507,7 +507,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C8">
         <v>0.345200271122541</v>

</xml_diff>

<commit_message>
Added a return target through a slider
We have now added a return target through incorporating a new slider for the return target value.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -429,7 +429,7 @@
         <v>3.876022766635678e-18</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.3467746958790734</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -443,7 +443,7 @@
         <v>0.02124815174069435</v>
       </c>
       <c r="D3">
-        <v>0.02124764584718219</v>
+        <v>0.3334176855470986</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -457,7 +457,7 @@
         <v>0.1273388301359862</v>
       </c>
       <c r="D4">
-        <v>0.1273383454430054</v>
+        <v>7.531898512759859e-19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -471,7 +471,7 @@
         <v>0.1697700754744735</v>
       </c>
       <c r="D5">
-        <v>0.1697703529919921</v>
+        <v>2.188874988996542e-19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -485,7 +485,7 @@
         <v>0.2390017860881791</v>
       </c>
       <c r="D6">
-        <v>0.2390020959213678</v>
+        <v>8.29629462328943e-19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -499,7 +499,7 @@
         <v>0.09744088543812593</v>
       </c>
       <c r="D7">
-        <v>0.09744157541012331</v>
+        <v>0.3077857311009995</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -513,7 +513,7 @@
         <v>0.345200271122541</v>
       </c>
       <c r="D8">
-        <v>0.3451999843863293</v>
+        <v>0.01202188747282855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Relocating the return_slider definition
We placed the definition of the return_slider to the top of the code, because it is required in a function that comes after it at that initial point hence, we get a "not defined" error.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0.3</v>
       </c>
       <c r="C2">
-        <v>3.876022766635678e-18</v>
+        <v>2.927345865710862e-18</v>
       </c>
       <c r="D2">
-        <v>0.3467746958790734</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.02124815174069435</v>
+        <v>0.02124717618409318</v>
       </c>
       <c r="D3">
-        <v>0.3334176855470986</v>
+        <v>0.02124715427314639</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,10 +454,10 @@
         <v>0.15</v>
       </c>
       <c r="C4">
-        <v>0.1273388301359862</v>
+        <v>0.1273382014015918</v>
       </c>
       <c r="D4">
-        <v>7.531898512759859e-19</v>
+        <v>0.1273388940376063</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.1697700754744735</v>
+        <v>0.1697704453391681</v>
       </c>
       <c r="D5">
-        <v>2.188874988996542e-19</v>
+        <v>0.1697699223641621</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +482,10 @@
         <v>0.1</v>
       </c>
       <c r="C6">
-        <v>0.2390017860881791</v>
+        <v>0.2390021039874927</v>
       </c>
       <c r="D6">
-        <v>8.29629462328943e-19</v>
+        <v>0.2390017823104368</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.05</v>
       </c>
       <c r="C7">
-        <v>0.09744088543812593</v>
+        <v>0.09744142026537399</v>
       </c>
       <c r="D7">
-        <v>0.3077857311009995</v>
+        <v>0.09744136897287403</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,10 +510,10 @@
         <v>0.1</v>
       </c>
       <c r="C8">
-        <v>0.345200271122541</v>
+        <v>0.34520065282228</v>
       </c>
       <c r="D8">
-        <v>0.01202188747282855</v>
+        <v>0.3452008780417743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix read excel all columns
We automated the reading process from the excel file. The code currently reads in all data from excel a well as the names of the financial products and then automatically outputs them on the figure.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Initial Weights</t>
   </si>
@@ -25,25 +25,28 @@
     <t>Opt Portfolio with View</t>
   </si>
   <si>
+    <t>thanos</t>
+  </si>
+  <si>
     <t>PARSTEI LX Equity</t>
   </si>
   <si>
-    <t>FLOT FP Equity</t>
-  </si>
-  <si>
-    <t>SX5EEX GY Equity</t>
-  </si>
-  <si>
-    <t>SPY US Equity</t>
-  </si>
-  <si>
-    <t>LFGGBDR LX Equity</t>
-  </si>
-  <si>
-    <t>EUN5 GY Equity</t>
-  </si>
-  <si>
-    <t>EUNH GY Equity</t>
+    <t>LEF1TREU Index</t>
+  </si>
+  <si>
+    <t>SX5R Index</t>
+  </si>
+  <si>
+    <t>SXUSR Index</t>
+  </si>
+  <si>
+    <t>BEGCGA Index</t>
+  </si>
+  <si>
+    <t>LEC4TREU Index</t>
+  </si>
+  <si>
+    <t>LEATTREU Index</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,10 +429,10 @@
         <v>0.3</v>
       </c>
       <c r="C2">
-        <v>2.927345865710862e-18</v>
+        <v>0.03595218056188074</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.0359521717459174</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +443,10 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.02124717618409318</v>
+        <v>0.1909876858665356</v>
       </c>
       <c r="D3">
-        <v>0.02124715427314639</v>
+        <v>0.1909876982079544</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,10 +457,10 @@
         <v>0.15</v>
       </c>
       <c r="C4">
-        <v>0.1273382014015918</v>
+        <v>0.1838869452973091</v>
       </c>
       <c r="D4">
-        <v>0.1273388940376063</v>
+        <v>0.1838869262343344</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +471,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.1697704453391681</v>
+        <v>0.07553560992936761</v>
       </c>
       <c r="D5">
-        <v>0.1697699223641621</v>
+        <v>0.0755356137722062</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +485,10 @@
         <v>0.1</v>
       </c>
       <c r="C6">
-        <v>0.2390021039874927</v>
+        <v>0.06451041465115818</v>
       </c>
       <c r="D6">
-        <v>0.2390017823104368</v>
+        <v>0.0645103867352906</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +499,10 @@
         <v>0.05</v>
       </c>
       <c r="C7">
-        <v>0.09744142026537399</v>
+        <v>0.1114101465131827</v>
       </c>
       <c r="D7">
-        <v>0.09744136897287403</v>
+        <v>0.111410190157718</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,13 +510,27 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C8">
-        <v>0.34520065282228</v>
+        <v>0.1699542531985195</v>
       </c>
       <c r="D8">
-        <v>0.3452008780417743</v>
+        <v>0.1699542547564113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0.05</v>
+      </c>
+      <c r="C9">
+        <v>0.1677627639820466</v>
+      </c>
+      <c r="D9">
+        <v>0.1677627583901678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new cell with sliders that contains new initial weights
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Initial Weights</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>Opt Portfolio with View</t>
-  </si>
-  <si>
-    <t>thanos</t>
   </si>
   <si>
     <t>PARSTEI LX Equity</t>
@@ -404,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,10 +426,10 @@
         <v>0.3</v>
       </c>
       <c r="C2">
-        <v>0.03595218056188074</v>
+        <v>2.927345865710862e-18</v>
       </c>
       <c r="D2">
-        <v>0.0359521717459174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -443,10 +440,10 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.1909876858665356</v>
+        <v>0.02124717618409318</v>
       </c>
       <c r="D3">
-        <v>0.1909876982079544</v>
+        <v>0.02124715427314639</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -457,10 +454,10 @@
         <v>0.15</v>
       </c>
       <c r="C4">
-        <v>0.1838869452973091</v>
+        <v>0.1273382014015918</v>
       </c>
       <c r="D4">
-        <v>0.1838869262343344</v>
+        <v>0.1273388940376063</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -471,10 +468,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.07553560992936761</v>
+        <v>0.1697704453391681</v>
       </c>
       <c r="D5">
-        <v>0.0755356137722062</v>
+        <v>0.1697699223641621</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -485,10 +482,10 @@
         <v>0.1</v>
       </c>
       <c r="C6">
-        <v>0.06451041465115818</v>
+        <v>0.2390021039874927</v>
       </c>
       <c r="D6">
-        <v>0.0645103867352906</v>
+        <v>0.2390017823104368</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -499,10 +496,10 @@
         <v>0.05</v>
       </c>
       <c r="C7">
-        <v>0.1114101465131827</v>
+        <v>0.09744142026537399</v>
       </c>
       <c r="D7">
-        <v>0.111410190157718</v>
+        <v>0.09744136897287403</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,27 +507,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C8">
-        <v>0.1699542531985195</v>
+        <v>0.34520065282228</v>
       </c>
       <c r="D8">
-        <v>0.1699542547564113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0.05</v>
-      </c>
-      <c r="C9">
-        <v>0.1677627639820466</v>
-      </c>
-      <c r="D9">
-        <v>0.1677627583901678</v>
+        <v>0.3452008780417743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial weight sliders working
We have created a new jupyter notebook cell where the user is asked to specify the initial weights of the portfolio. These are then passed on to the main code cell where they are utilised as the initial weights.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -423,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>2.927345865710862e-18</v>
+        <v>0.004410933559855143</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.0044109444566214</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -437,13 +437,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.02124717618409318</v>
+        <v>0.004352063267490375</v>
       </c>
       <c r="D3">
-        <v>0.02124715427314639</v>
+        <v>0.004352065352112043</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -451,13 +451,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.1273382014015918</v>
+        <v>0.3011493610815403</v>
       </c>
       <c r="D4">
-        <v>0.1273388940376063</v>
+        <v>0.3011490759015035</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -465,13 +465,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="C5">
-        <v>0.1697704453391681</v>
+        <v>0.678644535406819</v>
       </c>
       <c r="D5">
-        <v>0.1697699223641621</v>
+        <v>0.6786447681426276</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -479,13 +479,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="C6">
-        <v>0.2390021039874927</v>
+        <v>0.002944360464062921</v>
       </c>
       <c r="D6">
-        <v>0.2390017823104368</v>
+        <v>0.00294437259506601</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -493,13 +493,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>0.09744142026537399</v>
+        <v>0.004242739850924624</v>
       </c>
       <c r="D7">
-        <v>0.09744136897287403</v>
+        <v>0.00424274542942027</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,13 +507,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0.34520065282228</v>
+        <v>0.004256006369307748</v>
       </c>
       <c r="D8">
-        <v>0.3452008780417743</v>
+        <v>0.004256028122649053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Morphologically change the initial weight sliders and add text
We change the appearance of the initial weight sliders to have them correctly display the name of each asset without truncating it. We also added text description for each piece of code.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -423,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.448</v>
       </c>
       <c r="C2">
-        <v>0.004410933559855143</v>
+        <v>0.1295008802254504</v>
       </c>
       <c r="D2">
-        <v>0.0044109444566214</v>
+        <v>0.1295008734111448</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.004352063267490375</v>
+        <v>0.1316564287853225</v>
       </c>
       <c r="D3">
-        <v>0.004352065352112043</v>
+        <v>0.1316564464375971</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,10 +454,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.3011493610815403</v>
+        <v>0.004124283841947814</v>
       </c>
       <c r="D4">
-        <v>0.3011490759015035</v>
+        <v>0.004124274747723301</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -465,13 +465,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.678644535406819</v>
+        <v>1.061149016206822e-05</v>
       </c>
       <c r="D5">
-        <v>0.6786447681426276</v>
+        <v>1.060878357728654e-05</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -479,13 +479,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0.002944360464062921</v>
+        <v>0.006724954885701882</v>
       </c>
       <c r="D6">
-        <v>0.00294437259506601</v>
+        <v>0.006724945978417399</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -493,13 +493,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.346</v>
       </c>
       <c r="C7">
-        <v>0.004242739850924624</v>
+        <v>0.1327159474968135</v>
       </c>
       <c r="D7">
-        <v>0.00424274542942027</v>
+        <v>0.1327159446342338</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,13 +507,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.204</v>
       </c>
       <c r="C8">
-        <v>0.004256006369307748</v>
+        <v>0.5952668932746017</v>
       </c>
       <c r="D8">
-        <v>0.004256028122649053</v>
+        <v>0.5952669060073064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quick cleanup of code
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -423,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.448</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.1295008802254504</v>
+        <v>0.006839030729844959</v>
       </c>
       <c r="D2">
-        <v>0.1295008734111448</v>
+        <v>0.006839037839526434</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.1316564287853225</v>
+        <v>0.006063485726328331</v>
       </c>
       <c r="D3">
-        <v>0.1316564464375971</v>
+        <v>0.006063540109570382</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -451,13 +451,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.544</v>
       </c>
       <c r="C4">
-        <v>0.004124283841947814</v>
+        <v>0.3390115951598157</v>
       </c>
       <c r="D4">
-        <v>0.004124274747723301</v>
+        <v>0.3390118971693208</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1.061149016206822e-05</v>
+        <v>0.006451647308810614</v>
       </c>
       <c r="D5">
-        <v>1.060878357728654e-05</v>
+        <v>0.006451308842870747</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -479,13 +479,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C6">
-        <v>0.006724954885701882</v>
+        <v>0.6161722174184725</v>
       </c>
       <c r="D6">
-        <v>0.006724945978417399</v>
+        <v>0.6161721445573383</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.346</v>
       </c>
       <c r="C7">
-        <v>0.1327159474968135</v>
+        <v>0.006396234510063269</v>
       </c>
       <c r="D7">
-        <v>0.1327159446342338</v>
+        <v>0.006396328371717159</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,13 +507,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.204</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0.5952668932746017</v>
+        <v>0.01906578914666444</v>
       </c>
       <c r="D8">
-        <v>0.5952669060073064</v>
+        <v>0.0190657431096562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Current Layout seems to be what the user would expect.
We have re-arranged the figures towards the bottom of the notebook and placed the controls that control the "views" + "confidence_level" at the top.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.006839030729844959</v>
+        <v>0.009107798753669715</v>
       </c>
       <c r="D2">
-        <v>0.006839037839526434</v>
+        <v>0.009107790128166187</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.006063485726328331</v>
+        <v>0.009295874146037157</v>
       </c>
       <c r="D3">
-        <v>0.006063540109570382</v>
+        <v>0.009295884517358225</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -451,13 +451,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.544</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.3390115951598157</v>
+        <v>0.4522932122695642</v>
       </c>
       <c r="D4">
-        <v>0.3390118971693208</v>
+        <v>0.4522932116590938</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -465,13 +465,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="C5">
-        <v>0.006451647308810614</v>
+        <v>0.5030758649096663</v>
       </c>
       <c r="D5">
-        <v>0.006451308842870747</v>
+        <v>0.5030758693417202</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -479,13 +479,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.3</v>
+        <v>0.332</v>
       </c>
       <c r="C6">
-        <v>0.6161722174184725</v>
+        <v>0.007816705506625485</v>
       </c>
       <c r="D6">
-        <v>0.6161721445573383</v>
+        <v>0.007816689436843759</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -493,13 +493,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.346</v>
+        <v>0.342</v>
       </c>
       <c r="C7">
-        <v>0.006396234510063269</v>
+        <v>0.009388361714326349</v>
       </c>
       <c r="D7">
-        <v>0.006396328371717159</v>
+        <v>0.009388362662918238</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,13 +507,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.262</v>
       </c>
       <c r="C8">
-        <v>0.01906578914666444</v>
+        <v>0.00902218270011074</v>
       </c>
       <c r="D8">
-        <v>0.0190657431096562</v>
+        <v>0.009022192253899598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
same commit as before
Transfering the code to the terminal to see the effects of the change.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -25,25 +25,25 @@
     <t>Opt Portfolio with View</t>
   </si>
   <si>
-    <t>PARSTEI LX Equity</t>
-  </si>
-  <si>
-    <t>LEF1TREU Index</t>
-  </si>
-  <si>
-    <t>SX5R Index</t>
-  </si>
-  <si>
-    <t>SXUSR Index</t>
-  </si>
-  <si>
-    <t>BEGCGA Index</t>
-  </si>
-  <si>
-    <t>LEC4TREU Index</t>
-  </si>
-  <si>
-    <t>LEATTREU Index</t>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>EU Flot</t>
+  </si>
+  <si>
+    <t>EU Equity</t>
+  </si>
+  <si>
+    <t>US Equity</t>
+  </si>
+  <si>
+    <t>Greek Gov</t>
+  </si>
+  <si>
+    <t>EU Corps</t>
+  </si>
+  <si>
+    <t>EU Gov</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
         <v>0.1535818494881181</v>
       </c>
       <c r="D2">
-        <v>0.05951570120983125</v>
+        <v>0.1535818517403586</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -443,7 +443,7 @@
         <v>0.1522119935248375</v>
       </c>
       <c r="D3">
-        <v>0.05987609487342284</v>
+        <v>0.1522119952635631</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -457,7 +457,7 @@
         <v>0.1315750994568295</v>
       </c>
       <c r="D4">
-        <v>0.009253613110167381</v>
+        <v>0.1315750985927389</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -471,7 +471,7 @@
         <v>0.1316127757455861</v>
       </c>
       <c r="D5">
-        <v>0.06345261981704933</v>
+        <v>0.1316127758639908</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -485,7 +485,7 @@
         <v>0.1315393275253767</v>
       </c>
       <c r="D6">
-        <v>0.02027509981001521</v>
+        <v>0.1315393293010641</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -499,7 +499,7 @@
         <v>0.1495287230745071</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.149528721328849</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -513,7 +513,7 @@
         <v>0.149950231184745</v>
       </c>
       <c r="D8">
-        <v>0.787626871179514</v>
+        <v>0.1499502279094355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Supressing commit and general morphological
We delete the second tab in the POI that displayed the option to change the initial weights. However, due to our change of the program according to which we specify the weights in the previous cell this no longer works. Hence, we have now supressed it.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -423,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.1428571428571428</v>
+        <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.1535818494881181</v>
+        <v>0.1272849253007465</v>
       </c>
       <c r="D2">
-        <v>0.1535818517403586</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -437,13 +437,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.1428571428571428</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.1522119935248375</v>
+        <v>0.1272908224383453</v>
       </c>
       <c r="D3">
-        <v>0.1522119952635631</v>
+        <v>0.1163737759267746</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -451,13 +451,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1428571428571428</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
-        <v>0.1315750994568295</v>
+        <v>0.1796008618156742</v>
       </c>
       <c r="D4">
-        <v>0.1315750985927389</v>
+        <v>0.2176989893803725</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -465,13 +465,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.1428571428571428</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.1316127757455861</v>
+        <v>0.1722192567577291</v>
       </c>
       <c r="D5">
-        <v>0.1316127758639908</v>
+        <v>0.1949831861608918</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -479,13 +479,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.1428571428571428</v>
+        <v>0.15</v>
       </c>
       <c r="C6">
-        <v>0.1315393275253767</v>
+        <v>0.1389108338040999</v>
       </c>
       <c r="D6">
-        <v>0.1315393293010641</v>
+        <v>0.07649963773174576</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -493,13 +493,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.1428571428571428</v>
+        <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.1495287230745071</v>
+        <v>0.1272876650722808</v>
       </c>
       <c r="D7">
-        <v>0.149528721328849</v>
+        <v>0.223703413766908</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,13 +507,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.1428571428571428</v>
+        <v>0.3</v>
       </c>
       <c r="C8">
-        <v>0.149950231184745</v>
+        <v>0.1274056348111242</v>
       </c>
       <c r="D8">
-        <v>0.1499502279094355</v>
+        <v>0.1707409970333074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new cell to notebook
We added a new cell that enables the user to choose the frequency of the data that they input to the program. The user is given a choice of inputing daily, weekly, monthly data by choosing among three checkboxes.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -423,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C2">
-        <v>0.1272849253007465</v>
+        <v>0.1521569877763614</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.1521569873121236</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -437,13 +437,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.05</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C3">
-        <v>0.1272908224383453</v>
+        <v>0.1514628155394849</v>
       </c>
       <c r="D3">
-        <v>0.1163737759267746</v>
+        <v>0.1514628154088595</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -451,13 +451,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C4">
-        <v>0.1796008618156742</v>
+        <v>0.1307254289492208</v>
       </c>
       <c r="D4">
-        <v>0.2176989893803725</v>
+        <v>0.1307254287537006</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -465,13 +465,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C5">
-        <v>0.1722192567577291</v>
+        <v>0.1307357372099624</v>
       </c>
       <c r="D5">
-        <v>0.1949831861608918</v>
+        <v>0.130735737147938</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -479,13 +479,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.15</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C6">
-        <v>0.1389108338040999</v>
+        <v>0.1344673604747327</v>
       </c>
       <c r="D6">
-        <v>0.07649963773174576</v>
+        <v>0.1344673608767446</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -493,13 +493,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.2</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C7">
-        <v>0.1272876650722808</v>
+        <v>0.1501043822555428</v>
       </c>
       <c r="D7">
-        <v>0.223703413766908</v>
+        <v>0.1501043828279517</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,13 +507,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.3</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C8">
-        <v>0.1274056348111242</v>
+        <v>0.1503472877946951</v>
       </c>
       <c r="D8">
-        <v>0.1707409970333074</v>
+        <v>0.150347287672682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Applying the latest code (from previous commit) to terminal
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -423,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.1428571428571428</v>
+        <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.1521569877763614</v>
+        <v>0.1272849257335129</v>
       </c>
       <c r="D2">
-        <v>0.1521569873121236</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -437,13 +437,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.1428571428571428</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.1514628155394849</v>
+        <v>0.1272908228833229</v>
       </c>
       <c r="D3">
-        <v>0.1514628154088595</v>
+        <v>0.116373596538509</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -451,13 +451,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1428571428571428</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
-        <v>0.1307254289492208</v>
+        <v>0.1796008644373881</v>
       </c>
       <c r="D4">
-        <v>0.1307254287537006</v>
+        <v>0.2176989735329594</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -465,13 +465,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.1428571428571428</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.1307357372099624</v>
+        <v>0.1722192554824873</v>
       </c>
       <c r="D5">
-        <v>0.130735737147938</v>
+        <v>0.1949832312352888</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -479,13 +479,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.1428571428571428</v>
+        <v>0.15</v>
       </c>
       <c r="C6">
-        <v>0.1344673604747327</v>
+        <v>0.138910830905883</v>
       </c>
       <c r="D6">
-        <v>0.1344673608767446</v>
+        <v>0.07649952086827418</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -493,13 +493,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.1428571428571428</v>
+        <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.1501043822555428</v>
+        <v>0.1272876666956859</v>
       </c>
       <c r="D7">
-        <v>0.1501043828279517</v>
+        <v>0.2237036221345661</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,13 +507,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.1428571428571428</v>
+        <v>0.3</v>
       </c>
       <c r="C8">
-        <v>0.1503472877946951</v>
+        <v>0.1274056338617202</v>
       </c>
       <c r="D8">
-        <v>0.150347287672682</v>
+        <v>0.1707410556904025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes plus addition of environment yml file
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -429,7 +429,7 @@
         <v>0.1272849257335129</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.1272849253844004</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -443,7 +443,7 @@
         <v>0.1272908228833229</v>
       </c>
       <c r="D3">
-        <v>0.116373596538509</v>
+        <v>0.1272908219143504</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -457,7 +457,7 @@
         <v>0.1796008644373881</v>
       </c>
       <c r="D4">
-        <v>0.2176989735329594</v>
+        <v>0.1796008640945683</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -471,7 +471,7 @@
         <v>0.1722192554824873</v>
       </c>
       <c r="D5">
-        <v>0.1949832312352888</v>
+        <v>0.1722192543128125</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -485,7 +485,7 @@
         <v>0.138910830905883</v>
       </c>
       <c r="D6">
-        <v>0.07649952086827418</v>
+        <v>0.1389108337282178</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -499,7 +499,7 @@
         <v>0.1272876666956859</v>
       </c>
       <c r="D7">
-        <v>0.2237036221345661</v>
+        <v>0.1272876666760212</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -513,7 +513,7 @@
         <v>0.1274056338617202</v>
       </c>
       <c r="D8">
-        <v>0.1707410556904025</v>
+        <v>0.1274056338896295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new terminal that doesnt display code
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -423,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C2">
-        <v>0.1272849257335129</v>
+        <v>0.1535818480114002</v>
       </c>
       <c r="D2">
-        <v>0.1272849253844004</v>
+        <v>0.1535818492496737</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -437,13 +437,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.05</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C3">
-        <v>0.1272908228833229</v>
+        <v>0.1522119943432627</v>
       </c>
       <c r="D3">
-        <v>0.1272908219143504</v>
+        <v>0.1522119928421055</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -451,13 +451,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C4">
-        <v>0.1796008644373881</v>
+        <v>0.1315750976089232</v>
       </c>
       <c r="D4">
-        <v>0.1796008640945683</v>
+        <v>0.1315750984268254</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -465,13 +465,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C5">
-        <v>0.1722192554824873</v>
+        <v>0.1316127775234491</v>
       </c>
       <c r="D5">
-        <v>0.1722192543128125</v>
+        <v>0.1316127770923149</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -479,13 +479,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.15</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C6">
-        <v>0.138910830905883</v>
+        <v>0.1315393276269073</v>
       </c>
       <c r="D6">
-        <v>0.1389108337282178</v>
+        <v>0.1315393269293997</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -493,13 +493,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.2</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C7">
-        <v>0.1272876666956859</v>
+        <v>0.1495287225222207</v>
       </c>
       <c r="D7">
-        <v>0.1272876666760212</v>
+        <v>0.1495287223521467</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -507,13 +507,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.3</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C8">
-        <v>0.1274056338617202</v>
+        <v>0.1499502323638368</v>
       </c>
       <c r="D8">
-        <v>0.1274056338896295</v>
+        <v>0.1499502331075342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplifying the product notebook
We dumb down the notebook that will be displayed to clients. Clients are unable to specifically run the code so we hide code and place a button that automatically runs all cells when clicked on. This way the client will not have to specifically run all cell on their own.

We still need to link the initial weights sliders to the code.
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C2">
-        <v>0.1535818480114002</v>
+        <v>0.03398908557859916</v>
       </c>
       <c r="D2">
-        <v>0.1535818492496737</v>
+        <v>0.03398899316178236</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C3">
-        <v>0.1522119943432627</v>
+        <v>0.03326733264542253</v>
       </c>
       <c r="D3">
-        <v>0.1522119928421055</v>
+        <v>0.03326733196496505</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -451,13 +451,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1428571428571428</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0.1315750976089232</v>
+        <v>0.09196051005819827</v>
       </c>
       <c r="D4">
-        <v>0.1315750984268254</v>
+        <v>0.09196052048333501</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C5">
-        <v>0.1316127775234491</v>
+        <v>0.09359360785550738</v>
       </c>
       <c r="D5">
-        <v>0.1316127770923149</v>
+        <v>0.09359362526776671</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +482,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C6">
-        <v>0.1315393276269073</v>
+        <v>0.6494120724745848</v>
       </c>
       <c r="D6">
-        <v>0.1315393269293997</v>
+        <v>0.64941204950374</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C7">
-        <v>0.1495287225222207</v>
+        <v>0.03665620485808728</v>
       </c>
       <c r="D7">
-        <v>0.1495287223521467</v>
+        <v>0.03665631947025359</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,10 +510,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C8">
-        <v>0.1499502323638368</v>
+        <v>0.06112118652960059</v>
       </c>
       <c r="D8">
-        <v>0.1499502331075342</v>
+        <v>0.06112116014815723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding comments to the product notebook and code
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -426,10 +426,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C2">
-        <v>0.03398908557859916</v>
+        <v>0.0972481420361959</v>
       </c>
       <c r="D2">
-        <v>0.03398899316178236</v>
+        <v>0.09724811614937853</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,10 +440,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C3">
-        <v>0.03326733264542253</v>
+        <v>0.09649764182944713</v>
       </c>
       <c r="D3">
-        <v>0.03326733196496505</v>
+        <v>0.09649766910532863</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -451,13 +451,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.42</v>
       </c>
       <c r="C4">
-        <v>0.09196051005819827</v>
+        <v>0.1473185240024383</v>
       </c>
       <c r="D4">
-        <v>0.09196052048333501</v>
+        <v>0.1473185371538656</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -468,10 +468,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C5">
-        <v>0.09359360785550738</v>
+        <v>0.09898494248164209</v>
       </c>
       <c r="D5">
-        <v>0.09359362526776671</v>
+        <v>0.09898493358485361</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -482,10 +482,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C6">
-        <v>0.6494120724745848</v>
+        <v>0.3482936652637426</v>
       </c>
       <c r="D6">
-        <v>0.64941204950374</v>
+        <v>0.3482936594876294</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -496,10 +496,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C7">
-        <v>0.03665620485808728</v>
+        <v>0.09828707602528544</v>
       </c>
       <c r="D7">
-        <v>0.03665631947025359</v>
+        <v>0.09828711179714611</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -510,10 +510,10 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="C8">
-        <v>0.06112118652960059</v>
+        <v>0.1133700083612487</v>
       </c>
       <c r="D8">
-        <v>0.06112116014815723</v>
+        <v>0.1133699727217983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
current html file works with sliders only
the graphs do not display at all
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -1,75 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Initial Weights</t>
-  </si>
-  <si>
-    <t>Opt Portfolio</t>
-  </si>
-  <si>
-    <t>Opt Portfolio with View</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>EU Flot</t>
-  </si>
-  <si>
-    <t>EU Equity</t>
-  </si>
-  <si>
-    <t>US Equity</t>
-  </si>
-  <si>
-    <t>Greek Gov</t>
-  </si>
-  <si>
-    <t>EU Corps</t>
-  </si>
-  <si>
-    <t>EU Gov</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,18 +46,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -103,16 +57,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -400,123 +421,149 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0.1428571428571428</v>
-      </c>
-      <c r="C2">
-        <v>0.1535818494881181</v>
-      </c>
-      <c r="D2">
-        <v>0.1535818517403586</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>0.1428571428571428</v>
-      </c>
-      <c r="C3">
-        <v>0.1522119935248375</v>
-      </c>
-      <c r="D3">
-        <v>0.1522119952635631</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>0.1428571428571428</v>
-      </c>
-      <c r="C4">
-        <v>0.1315750994568295</v>
-      </c>
-      <c r="D4">
-        <v>0.1315750985927389</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.1428571428571428</v>
-      </c>
-      <c r="C5">
-        <v>0.1316127757455861</v>
-      </c>
-      <c r="D5">
-        <v>0.1316127758639908</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>0.1428571428571428</v>
-      </c>
-      <c r="C6">
-        <v>0.1315393275253767</v>
-      </c>
-      <c r="D6">
-        <v>0.1315393293010641</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0.1428571428571428</v>
-      </c>
-      <c r="C7">
-        <v>0.1495287230745071</v>
-      </c>
-      <c r="D7">
-        <v>0.149528721328849</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0.1428571428571428</v>
-      </c>
-      <c r="C8">
-        <v>0.149950231184745</v>
-      </c>
-      <c r="D8">
-        <v>0.1499502279094355</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Initial Weights</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Opt Portfolio</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Opt Portfolio with View</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1535818504135633</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1535818512568701</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>EU Flot</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1522119927096501</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1522119933428666</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>EU Equity</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.131575098567263</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.131575099332171</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>US Equity</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.13161277638873</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1316127768341236</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Greek Gov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.131539328051003</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1315393259675999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>EU Corps</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1495287229867142</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.149528723519125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>EU Gov</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1499502308830764</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.1499502297472438</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
current code is what works on local notebook programme
this code does not work at all on html, only on local notebook
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -464,7 +464,7 @@
         <v>0.1535818504135633</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1535818512568701</v>
+        <v>5.075712372040022e-17</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>0.1522119927096501</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1522119933428666</v>
+        <v>6.175624517019239e-17</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +496,7 @@
         <v>0.131575098567263</v>
       </c>
       <c r="D4" t="n">
-        <v>0.131575099332171</v>
+        <v>0.1389898938418274</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +512,7 @@
         <v>0.13161277638873</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1316127768341236</v>
+        <v>0.131042139217673</v>
       </c>
     </row>
     <row r="6">
@@ -528,7 +528,7 @@
         <v>0.131539328051003</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1315393259675999</v>
+        <v>0.09787673297163955</v>
       </c>
     </row>
     <row r="7">
@@ -544,7 +544,7 @@
         <v>0.1495287229867142</v>
       </c>
       <c r="D7" t="n">
-        <v>0.149528723519125</v>
+        <v>0.6320912339688598</v>
       </c>
     </row>
     <row r="8">
@@ -560,7 +560,7 @@
         <v>0.1499502308830764</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1499502297472438</v>
+        <v>6.24064294285224e-17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Current html files print a graph (but not ours)
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -464,7 +464,7 @@
         <v>0.1535818504135633</v>
       </c>
       <c r="D2" t="n">
-        <v>5.075712372040022e-17</v>
+        <v>0.1535818512568701</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>0.1522119927096501</v>
       </c>
       <c r="D3" t="n">
-        <v>6.175624517019239e-17</v>
+        <v>0.1522119933428666</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +496,7 @@
         <v>0.131575098567263</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1389898938418274</v>
+        <v>0.131575099332171</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +512,7 @@
         <v>0.13161277638873</v>
       </c>
       <c r="D5" t="n">
-        <v>0.131042139217673</v>
+        <v>0.1316127768341236</v>
       </c>
     </row>
     <row r="6">
@@ -528,7 +528,7 @@
         <v>0.131539328051003</v>
       </c>
       <c r="D6" t="n">
-        <v>0.09787673297163955</v>
+        <v>0.1315393259675999</v>
       </c>
     </row>
     <row r="7">
@@ -544,7 +544,7 @@
         <v>0.1495287229867142</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6320912339688598</v>
+        <v>0.149528723519125</v>
       </c>
     </row>
     <row r="8">
@@ -560,7 +560,7 @@
         <v>0.1499502308830764</v>
       </c>
       <c r="D8" t="n">
-        <v>6.24064294285224e-17</v>
+        <v>0.1499502297472438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Current configuration works great in Firefox, Safari
the current product.html file works as expected in safari and firefox!
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -464,7 +464,7 @@
         <v>0.1535818504135633</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1535818512568701</v>
+        <v>0.0004904227247809496</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>0.1522119927096501</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1522119933428666</v>
+        <v>1.923671547856839e-17</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +496,7 @@
         <v>0.131575098567263</v>
       </c>
       <c r="D4" t="n">
-        <v>0.131575099332171</v>
+        <v>0.05740214944097932</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +512,7 @@
         <v>0.13161277638873</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1316127768341236</v>
+        <v>0.04284130731152905</v>
       </c>
     </row>
     <row r="6">
@@ -528,7 +528,7 @@
         <v>0.131539328051003</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1315393259675999</v>
+        <v>0.0446838664608151</v>
       </c>
     </row>
     <row r="7">
@@ -544,7 +544,7 @@
         <v>0.1495287229867142</v>
       </c>
       <c r="D7" t="n">
-        <v>0.149528723519125</v>
+        <v>0.8545822540618956</v>
       </c>
     </row>
     <row r="8">
@@ -560,7 +560,7 @@
         <v>0.1499502308830764</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1499502297472438</v>
+        <v>5.24531075531447e-18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
We delete the extra graph used for checking
we delete the plotting of a "test" graph at the start of the code!
</commit_message>
<xml_diff>
--- a/Main/output.xlsx
+++ b/Main/output.xlsx
@@ -464,7 +464,7 @@
         <v>0.1535818504135633</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0004904227247809496</v>
+        <v>0.1535818512568701</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>0.1522119927096501</v>
       </c>
       <c r="D3" t="n">
-        <v>1.923671547856839e-17</v>
+        <v>0.1522119933428666</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +496,7 @@
         <v>0.131575098567263</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05740214944097932</v>
+        <v>0.131575099332171</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +512,7 @@
         <v>0.13161277638873</v>
       </c>
       <c r="D5" t="n">
-        <v>0.04284130731152905</v>
+        <v>0.1316127768341236</v>
       </c>
     </row>
     <row r="6">
@@ -528,7 +528,7 @@
         <v>0.131539328051003</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0446838664608151</v>
+        <v>0.1315393259675999</v>
       </c>
     </row>
     <row r="7">
@@ -544,7 +544,7 @@
         <v>0.1495287229867142</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8545822540618956</v>
+        <v>0.149528723519125</v>
       </c>
     </row>
     <row r="8">
@@ -560,7 +560,7 @@
         <v>0.1499502308830764</v>
       </c>
       <c r="D8" t="n">
-        <v>5.24531075531447e-18</v>
+        <v>0.1499502297472438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>